<commit_message>
develop-master : fix import karyawan
</commit_message>
<xml_diff>
--- a/public/template_import.xlsx
+++ b/public/template_import.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tole\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project\Laravel\bio_interface\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE001F21-4A61-446C-A916-4FB36D84985C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="52">
   <si>
     <t>nip</t>
   </si>
@@ -159,12 +160,33 @@
   </si>
   <si>
     <t>stf1</t>
+  </si>
+  <si>
+    <t>kd_entitas</t>
+  </si>
+  <si>
+    <t>status_jabatan</t>
+  </si>
+  <si>
+    <t>kd_bagian</t>
+  </si>
+  <si>
+    <t>pendidikan</t>
+  </si>
+  <si>
+    <t>tgl_mulai</t>
+  </si>
+  <si>
+    <t>tanggal_penonaktifan</t>
+  </si>
+  <si>
+    <t>sk_pemberhentian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -217,7 +239,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -498,41 +520,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="15" customWidth="1"/>
+    <col min="25" max="26" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,70 +569,91 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1234</v>
       </c>
@@ -616,65 +663,65 @@
       <c r="C2">
         <v>3511112</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>41</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="2">
+      <c r="O2" s="2">
         <v>37551</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>25</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>31</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>32</v>
       </c>
-      <c r="R2" t="s">
+      <c r="Y2" t="s">
         <v>27</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Z2" t="s">
         <v>28</v>
       </c>
-      <c r="T2">
+      <c r="AA2">
         <v>2000000</v>
       </c>
-      <c r="U2">
+      <c r="AB2">
         <v>2000000</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AC2" t="s">
         <v>29</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AD2" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="2">
+      <c r="AE2" s="2">
         <v>42299</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1235</v>
       </c>
@@ -684,65 +731,65 @@
       <c r="C3">
         <v>3511113</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>40</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>44</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>41</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="2">
+      <c r="O3" s="2">
         <v>37551</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>25</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>31</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>32</v>
       </c>
-      <c r="R3" t="s">
+      <c r="Y3" t="s">
         <v>27</v>
       </c>
-      <c r="S3" t="s">
+      <c r="Z3" t="s">
         <v>28</v>
       </c>
-      <c r="T3">
+      <c r="AA3">
         <v>2000000</v>
       </c>
-      <c r="U3">
+      <c r="AB3">
         <v>2000000</v>
       </c>
-      <c r="V3" t="s">
+      <c r="AC3" t="s">
         <v>29</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AD3" t="s">
         <v>30</v>
       </c>
-      <c r="X3" s="2">
+      <c r="AE3" s="2">
         <v>42299</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1236</v>
       </c>
@@ -752,65 +799,65 @@
       <c r="C4">
         <v>3511114</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>39</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>44</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
         <v>22</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="2">
+      <c r="O4" s="2">
         <v>37551</v>
       </c>
-      <c r="M4" t="s">
+      <c r="P4" t="s">
         <v>24</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>25</v>
       </c>
-      <c r="O4" t="s">
+      <c r="R4" t="s">
         <v>31</v>
       </c>
-      <c r="P4" t="s">
+      <c r="S4" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>32</v>
       </c>
-      <c r="R4" t="s">
+      <c r="Y4" t="s">
         <v>27</v>
       </c>
-      <c r="S4" t="s">
+      <c r="Z4" t="s">
         <v>28</v>
       </c>
-      <c r="T4">
+      <c r="AA4">
         <v>2000000</v>
       </c>
-      <c r="U4">
+      <c r="AB4">
         <v>2000000</v>
       </c>
-      <c r="V4" t="s">
+      <c r="AC4" t="s">
         <v>29</v>
       </c>
-      <c r="W4" t="s">
+      <c r="AD4" t="s">
         <v>30</v>
       </c>
-      <c r="X4" s="2">
+      <c r="AE4" s="2">
         <v>42299</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1237</v>
       </c>
@@ -820,65 +867,65 @@
       <c r="C5">
         <v>3511115</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>40</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>44</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>41</v>
       </c>
-      <c r="J5" t="s">
+      <c r="M5" t="s">
         <v>22</v>
       </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="2">
+      <c r="O5" s="2">
         <v>37551</v>
       </c>
-      <c r="M5" t="s">
+      <c r="P5" t="s">
         <v>24</v>
       </c>
-      <c r="N5" t="s">
+      <c r="Q5" t="s">
         <v>25</v>
       </c>
-      <c r="O5" t="s">
+      <c r="R5" t="s">
         <v>31</v>
       </c>
-      <c r="P5" t="s">
+      <c r="S5" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="T5" t="s">
         <v>32</v>
       </c>
-      <c r="R5" t="s">
+      <c r="Y5" t="s">
         <v>27</v>
       </c>
-      <c r="S5" t="s">
+      <c r="Z5" t="s">
         <v>28</v>
       </c>
-      <c r="T5">
+      <c r="AA5">
         <v>2000000</v>
       </c>
-      <c r="U5">
+      <c r="AB5">
         <v>2000000</v>
       </c>
-      <c r="V5" t="s">
+      <c r="AC5" t="s">
         <v>29</v>
       </c>
-      <c r="W5" t="s">
+      <c r="AD5" t="s">
         <v>30</v>
       </c>
-      <c r="X5" s="2">
+      <c r="AE5" s="2">
         <v>42299</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1238</v>
       </c>
@@ -888,61 +935,61 @@
       <c r="C6">
         <v>3511116</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>39</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>44</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>41</v>
       </c>
-      <c r="J6" t="s">
+      <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="K6" t="s">
+      <c r="N6" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="2">
+      <c r="O6" s="2">
         <v>37551</v>
       </c>
-      <c r="M6" t="s">
+      <c r="P6" t="s">
         <v>24</v>
       </c>
-      <c r="N6" t="s">
+      <c r="Q6" t="s">
         <v>25</v>
       </c>
-      <c r="O6" t="s">
+      <c r="R6" t="s">
         <v>31</v>
       </c>
-      <c r="P6" t="s">
+      <c r="S6" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="T6" t="s">
         <v>32</v>
       </c>
-      <c r="R6" t="s">
+      <c r="Y6" t="s">
         <v>27</v>
       </c>
-      <c r="S6" t="s">
+      <c r="Z6" t="s">
         <v>28</v>
       </c>
-      <c r="T6">
+      <c r="AA6">
         <v>2000000</v>
       </c>
-      <c r="U6">
+      <c r="AB6">
         <v>2000000</v>
       </c>
-      <c r="V6" t="s">
+      <c r="AC6" t="s">
         <v>29</v>
       </c>
-      <c r="W6" t="s">
+      <c r="AD6" t="s">
         <v>30</v>
       </c>
-      <c r="X6" s="2">
+      <c r="AE6" s="2">
         <v>42299</v>
       </c>
     </row>

</xml_diff>